<commit_message>
Se añaden los casos de prueba
</commit_message>
<xml_diff>
--- a/Reto pruebas manuales/Plan de pruebas.xlsx
+++ b/Reto pruebas manuales/Plan de pruebas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunez\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunez\Escritorio\Reto pruebas manuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2437A-5198-46C8-ADD3-2BD2546B7CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6D46EE-D779-40CC-AC57-EEE42166FFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Externo</t>
-  </si>
-  <si>
-    <t>Estudiante de Sofka U</t>
   </si>
   <si>
     <t>Release</t>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>Se probara el funcionamiento correcto de la web en las funcionalidades asociadas al flujo de compra utilizando una cuenta previamente creada y por medio de pruebas manuales en las cuales se realizaran distintos casos de prueba previamente diseñados.</t>
+  </si>
+  <si>
+    <t>José Nuñez</t>
   </si>
 </sst>
 </file>
@@ -795,7 +795,9 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1007,43 +1009,43 @@
     </row>
     <row r="7" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>15</v>
+      <c r="F7" s="19" t="s">
+        <v>19</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>23</v>
+      <c r="K7" s="10" t="s">
+        <v>28</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="M7" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1061,43 +1063,43 @@
     </row>
     <row r="8" spans="1:26" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="F8" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="10" t="s">
+      <c r="L8" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="24" t="s">
-        <v>30</v>
-      </c>
       <c r="M8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1115,43 +1117,43 @@
     </row>
     <row r="9" spans="1:26" ht="129.6" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>15</v>
+      <c r="F9" s="27" t="s">
+        <v>34</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="G9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="H9" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="I9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="10" t="s">
+      <c r="K9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="29" t="s">
-        <v>39</v>
-      </c>
       <c r="L9" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M9" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>

</xml_diff>